<commit_message>
SC version of CPT automation
</commit_message>
<xml_diff>
--- a/Input_files/Python_Multiple-CPT_Input_Template.xlsx
+++ b/Input_files/Python_Multiple-CPT_Input_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amb\PycharmProjects\SI_processing_automation\Input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sc\PycharmProjects\SI_processing_automation\Input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91339E5-3298-43E9-B0FE-E7561B158A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6605725-AA04-48F6-97C7-FD0179D17542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global_variable" sheetId="3" r:id="rId1"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="191">
   <si>
     <t>Figure folder path</t>
   </si>
@@ -188,39 +188,12 @@
     <t>Figure_extension</t>
   </si>
   <si>
-    <t>.svg</t>
-  </si>
-  <si>
-    <t>Thor_Fugro-2022-SI.gpj</t>
-  </si>
-  <si>
     <t>Units</t>
   </si>
   <si>
     <t>Color</t>
   </si>
   <si>
-    <t>U40-SAND</t>
-  </si>
-  <si>
-    <t>U46-CLAY</t>
-  </si>
-  <si>
-    <t>U98-CLAY</t>
-  </si>
-  <si>
-    <t>U98-SAND</t>
-  </si>
-  <si>
-    <t>#E0D68D</t>
-  </si>
-  <si>
-    <t>#228833</t>
-  </si>
-  <si>
-    <t>#802659</t>
-  </si>
-  <si>
     <t>SCPT location 1</t>
   </si>
   <si>
@@ -236,90 +209,6 @@
     <t>Processed data file name</t>
   </si>
   <si>
-    <t>U10-SAND</t>
-  </si>
-  <si>
-    <t>U13-CLAY</t>
-  </si>
-  <si>
-    <t>U13-SAND</t>
-  </si>
-  <si>
-    <t>U20-CLAY</t>
-  </si>
-  <si>
-    <t>U20-SAND</t>
-  </si>
-  <si>
-    <t>U20-SILT</t>
-  </si>
-  <si>
-    <t>U21-SAND</t>
-  </si>
-  <si>
-    <t>U30-CLAY</t>
-  </si>
-  <si>
-    <t>U30-SAND</t>
-  </si>
-  <si>
-    <t>U46-SAND</t>
-  </si>
-  <si>
-    <t>U47-CLAY</t>
-  </si>
-  <si>
-    <t>U50-CLAY</t>
-  </si>
-  <si>
-    <t>U50-SAND</t>
-  </si>
-  <si>
-    <t>U50-SILT</t>
-  </si>
-  <si>
-    <t>U59-CLAY</t>
-  </si>
-  <si>
-    <t>U99-CLAY</t>
-  </si>
-  <si>
-    <t>U99-SAND</t>
-  </si>
-  <si>
-    <t>U99-SILT</t>
-  </si>
-  <si>
-    <t>#cceaca</t>
-  </si>
-  <si>
-    <t>#ffd6eb</t>
-  </si>
-  <si>
-    <t>#661100</t>
-  </si>
-  <si>
-    <t>#b5725c</t>
-  </si>
-  <si>
-    <t>#ffd5c5</t>
-  </si>
-  <si>
-    <t>#332288</t>
-  </si>
-  <si>
-    <t>#9479c2</t>
-  </si>
-  <si>
-    <t>#ebdbff</t>
-  </si>
-  <si>
-    <t>#EE7733</t>
-  </si>
-  <si>
-    <t>#0077BB</t>
-  </si>
-  <si>
     <t>#efe3b5</t>
   </si>
   <si>
@@ -338,39 +227,6 @@
     <t>#b0ebff</t>
   </si>
   <si>
-    <t>#CC6677</t>
-  </si>
-  <si>
-    <t>#ffd2d9</t>
-  </si>
-  <si>
-    <t>#e4e6b7</t>
-  </si>
-  <si>
-    <t>S:\Clients\T-Z\Thor Wind Farm\02_Working\CPT-data\WTG\WTG-BH-41</t>
-  </si>
-  <si>
-    <t>S:\Clients\T-Z\Thor Wind Farm\02_Working\CPT-data\WTG\WTG-BH-41\CPT-fig</t>
-  </si>
-  <si>
-    <t>S:\Clients\T-Z\Thor Wind Farm\02_Working\CPT-data\WTG\WTG-BH-53\CPT-fig</t>
-  </si>
-  <si>
-    <t>WTG-BH-41_CPT_processed_data.csv</t>
-  </si>
-  <si>
-    <t>WTG-BH-53_CPT_processed_data.csv</t>
-  </si>
-  <si>
-    <t>WTG-BH-41</t>
-  </si>
-  <si>
-    <t>S:\Clients\T-Z\Thor Wind Farm\02_Working\CPT-data\WTG\WTG-BH-53</t>
-  </si>
-  <si>
-    <t>WTG-BH-53</t>
-  </si>
-  <si>
     <t>series name</t>
   </si>
   <si>
@@ -732,13 +588,133 @@
   </si>
   <si>
     <t>r'Jardine et al. (2005)'</t>
+  </si>
+  <si>
+    <t>.png</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Input_files\cpt_data_files\RWE-Taiwan</t>
+  </si>
+  <si>
+    <t>SCPT-combined.xlsx</t>
+  </si>
+  <si>
+    <t>SOIL_UNIT-combined.xlsx</t>
+  </si>
+  <si>
+    <t>Hsinchu-BH1-CPT_processed_data.csv</t>
+  </si>
+  <si>
+    <t>Hsinchu-BH3-CPT_processed_data.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\Processed-CPT\Hsinchu</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH01</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH03</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH04</t>
+  </si>
+  <si>
+    <t>SCPG-combined.xlsx</t>
+  </si>
+  <si>
+    <t>SOIL_PROPERTY-combined.xlsx</t>
+  </si>
+  <si>
+    <t>Hsinchu-BH4-CPT_processed_data.csv</t>
+  </si>
+  <si>
+    <t>BH01-HSINCHU</t>
+  </si>
+  <si>
+    <t>BH03-HSINCHU</t>
+  </si>
+  <si>
+    <t>BH04-HSINCHU</t>
+  </si>
+  <si>
+    <t>Clay</t>
+  </si>
+  <si>
+    <t>Sand</t>
+  </si>
+  <si>
+    <t>Sandy Clay</t>
+  </si>
+  <si>
+    <t>Silty Sand</t>
+  </si>
+  <si>
+    <t>Silt</t>
+  </si>
+  <si>
+    <t>Clayey Sand</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH02</t>
+  </si>
+  <si>
+    <t>Hsinchu-BH2-CPT_processed_data.csv</t>
+  </si>
+  <si>
+    <t>BH02-HSINCHU</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH05</t>
+  </si>
+  <si>
+    <t>Hsinchu-BH5-CPT_processed_data.csv</t>
+  </si>
+  <si>
+    <t>BH05-HSINCHU</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH06</t>
+  </si>
+  <si>
+    <t>Hsinchu-BH6-CPT_processed_data.csv</t>
+  </si>
+  <si>
+    <t>BH06-HSINCHU</t>
+  </si>
+  <si>
+    <t>Silty Clay</t>
+  </si>
+  <si>
+    <t>#99FF99</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH07</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH08</t>
+  </si>
+  <si>
+    <t>BH07-HSINCHU</t>
+  </si>
+  <si>
+    <t>BH08-HSINCHU</t>
+  </si>
+  <si>
+    <t>Sandy Silt</t>
+  </si>
+  <si>
+    <t>#CCCC00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -772,6 +748,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -781,7 +769,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -804,25 +792,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal_Sheet1" xfId="1" xr:uid="{766AB24F-1C03-4FDB-81C9-CE1DFEF48324}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1103,8 +1122,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,111 +1146,117 @@
     <col min="19" max="22" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" s="2" t="s">
+      <c r="O1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>31</v>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>70</v>
+      <c r="A2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="F2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G2" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" t="b">
-        <v>0</v>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5" t="s">
-        <v>73</v>
+      <c r="G2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="P2">
         <v>10</v>
@@ -1239,47 +1264,59 @@
       <c r="Q2">
         <v>0</v>
       </c>
-      <c r="R2" s="5" t="s">
-        <v>75</v>
+      <c r="R2" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="S2" t="s">
+        <v>166</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>76</v>
+      <c r="A3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5" t="s">
-        <v>74</v>
+      <c r="G3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="P3">
         <v>10</v>
@@ -1287,42 +1324,344 @@
       <c r="Q3">
         <v>0</v>
       </c>
-      <c r="R3" s="5" t="s">
-        <v>77</v>
+      <c r="R3" s="3" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="P4">
+        <v>10</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="P5">
+        <v>10</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5" t="s">
+        <v>176</v>
+      </c>
+      <c r="S5" t="s">
+        <v>179</v>
+      </c>
+      <c r="T5" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="P6">
+        <v>10</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="A7" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="P7">
+        <v>10</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7" t="s">
+        <v>182</v>
+      </c>
+      <c r="S7" t="s">
+        <v>187</v>
+      </c>
+      <c r="T7" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="A8" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="P8">
+        <v>10</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="P9">
+        <v>10</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -1335,10 +1674,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97D0C77-CF34-4830-A02F-345B9F600E1D}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,187 +1687,78 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
+      <c r="A2" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>34</v>
+      <c r="A3" s="6" t="s">
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>35</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>36</v>
+      <c r="A5" s="6" t="s">
+        <v>171</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>37</v>
+      <c r="A6" s="6" t="s">
+        <v>172</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>38</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>173</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>39</v>
+      <c r="A8" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>40</v>
+      <c r="A9" s="7" t="s">
+        <v>189</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" t="s">
-        <v>51</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" t="s">
-        <v>54</v>
-      </c>
+      <c r="B14" s="4"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B23">
@@ -1557,376 +1787,376 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
-        <v>138</v>
+        <v>90</v>
       </c>
       <c r="E1" t="s">
-        <v>128</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="A2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>92</v>
+        <v>32</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="5">
+        <v>76</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>93</v>
+        <v>33</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="5">
+        <v>77</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="5">
+        <v>122</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>95</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>63</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>37</v>
       </c>
       <c r="E7" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="C8">
         <v>1E-3</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>190</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>65</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="E9" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>191</v>
+        <v>143</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>66</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>192</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>133</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>193</v>
+        <v>145</v>
       </c>
       <c r="B12" t="s">
-        <v>107</v>
+        <v>59</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
+        <v>82</v>
       </c>
       <c r="E12" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>146</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>67</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>131</v>
+        <v>83</v>
       </c>
       <c r="E13" t="s">
-        <v>135</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>195</v>
+        <v>147</v>
       </c>
       <c r="B14" t="s">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>132</v>
+        <v>84</v>
       </c>
       <c r="E14" t="s">
-        <v>136</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>127</v>
       </c>
       <c r="B15" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>91</v>
+        <v>43</v>
       </c>
       <c r="E15" t="s">
-        <v>149</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>116</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
-        <v>116</v>
+        <v>68</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>140</v>
+        <v>92</v>
       </c>
       <c r="E16" t="s">
-        <v>139</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>69</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>141</v>
+        <v>93</v>
       </c>
       <c r="E17" t="s">
-        <v>145</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="B18" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>94</v>
       </c>
       <c r="E18" t="s">
-        <v>146</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>143</v>
+        <v>95</v>
       </c>
       <c r="E19" t="s">
-        <v>147</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>144</v>
+        <v>96</v>
       </c>
       <c r="E20" t="s">
-        <v>148</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>121</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>121</v>
+        <v>73</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="E21" t="s">
-        <v>197</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>122</v>
+        <v>74</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>198</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -1953,129 +2183,129 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>177</v>
+        <v>129</v>
       </c>
       <c r="C1" t="s">
-        <v>178</v>
+        <v>130</v>
       </c>
       <c r="D1" t="s">
-        <v>186</v>
+        <v>138</v>
       </c>
       <c r="E1" t="s">
-        <v>152</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s">
-        <v>168</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>153</v>
+        <v>128</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
       <c r="E3" t="s">
-        <v>154</v>
+        <v>106</v>
       </c>
       <c r="F3" t="s">
-        <v>161</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>107</v>
       </c>
       <c r="F4" t="s">
-        <v>162</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>55</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
       <c r="E5" t="s">
-        <v>156</v>
+        <v>108</v>
       </c>
       <c r="F5" t="s">
-        <v>163</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>123</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
       <c r="E6" t="s">
-        <v>151</v>
+        <v>103</v>
       </c>
       <c r="F6" t="s">
-        <v>164</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>124</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
       <c r="E7" t="s">
-        <v>157</v>
+        <v>109</v>
       </c>
       <c r="F7" t="s">
-        <v>165</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>125</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2084,32 +2314,32 @@
         <v>120</v>
       </c>
       <c r="E8" t="s">
-        <v>158</v>
+        <v>110</v>
       </c>
       <c r="F8" t="s">
-        <v>166</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>126</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
       <c r="E9" t="s">
-        <v>159</v>
+        <v>111</v>
       </c>
       <c r="F9" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>175</v>
+        <v>127</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -2118,10 +2348,10 @@
         <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
       <c r="F10" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2135,7 +2365,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
@@ -2152,103 +2382,103 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>183</v>
+        <v>135</v>
       </c>
       <c r="C1" t="s">
-        <v>196</v>
+        <v>148</v>
       </c>
       <c r="D1" t="s">
-        <v>184</v>
+        <v>136</v>
       </c>
       <c r="E1" t="s">
-        <v>185</v>
+        <v>137</v>
       </c>
       <c r="F1" t="s">
-        <v>187</v>
+        <v>139</v>
       </c>
       <c r="G1" t="s">
-        <v>188</v>
+        <v>140</v>
       </c>
       <c r="H1" t="s">
-        <v>189</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
-        <v>0</v>
-      </c>
-      <c r="B2" s="8">
+      <c r="A2" s="5">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
         <v>0</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>101</v>
+      <c r="D2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="G2" t="s">
-        <v>181</v>
+        <v>133</v>
       </c>
       <c r="H2" t="s">
-        <v>182</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
-        <v>0</v>
-      </c>
-      <c r="B3" s="8">
+      <c r="A3" s="5">
+        <v>0</v>
+      </c>
+      <c r="B3" s="5">
         <v>1</v>
       </c>
       <c r="C3" t="b">
         <v>1</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>170</v>
+      <c r="D3" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -2262,7 +2492,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2276,25 +2506,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
-        <v>196</v>
+        <v>148</v>
       </c>
       <c r="C1" t="s">
-        <v>184</v>
+        <v>136</v>
       </c>
       <c r="D1" t="s">
-        <v>185</v>
+        <v>137</v>
       </c>
       <c r="E1" t="s">
-        <v>187</v>
+        <v>139</v>
       </c>
       <c r="F1" t="s">
-        <v>188</v>
+        <v>140</v>
       </c>
       <c r="G1" t="s">
-        <v>189</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2305,19 +2535,19 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="E2" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>124</v>
+        <v>76</v>
       </c>
       <c r="G2" t="s">
-        <v>125</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2328,13 +2558,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>127</v>
       </c>
       <c r="D3" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="E3" t="s">
-        <v>175</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2345,16 +2575,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>172</v>
+        <v>124</v>
       </c>
       <c r="D4" t="s">
-        <v>169</v>
+        <v>121</v>
       </c>
       <c r="E4" t="s">
-        <v>190</v>
+        <v>142</v>
       </c>
       <c r="F4" t="s">
-        <v>191</v>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing the input excel file
</commit_message>
<xml_diff>
--- a/Input_files/Python_Multiple-CPT_Input_Template.xlsx
+++ b/Input_files/Python_Multiple-CPT_Input_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sc\PycharmProjects\SI_processing_automation\Input_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6605725-AA04-48F6-97C7-FD0179D17542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2E35D8-28D6-46B5-88D4-C8C39616895E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22500" yWindow="3690" windowWidth="18900" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global_variable" sheetId="3" r:id="rId1"/>
@@ -593,12 +593,6 @@
     <t>.png</t>
   </si>
   <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Input_files\cpt_data_files\RWE-Taiwan</t>
-  </si>
-  <si>
     <t>SCPT-combined.xlsx</t>
   </si>
   <si>
@@ -611,18 +605,6 @@
     <t>Hsinchu-BH3-CPT_processed_data.csv</t>
   </si>
   <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\Processed-CPT\Hsinchu</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH01</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH03</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH04</t>
-  </si>
-  <si>
     <t>SCPG-combined.xlsx</t>
   </si>
   <si>
@@ -659,27 +641,18 @@
     <t>Clayey Sand</t>
   </si>
   <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH02</t>
-  </si>
-  <si>
     <t>Hsinchu-BH2-CPT_processed_data.csv</t>
   </si>
   <si>
     <t>BH02-HSINCHU</t>
   </si>
   <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH05</t>
-  </si>
-  <si>
     <t>Hsinchu-BH5-CPT_processed_data.csv</t>
   </si>
   <si>
     <t>BH05-HSINCHU</t>
   </si>
   <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH06</t>
-  </si>
-  <si>
     <t>Hsinchu-BH6-CPT_processed_data.csv</t>
   </si>
   <si>
@@ -692,12 +665,6 @@
     <t>#99FF99</t>
   </si>
   <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH07</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH08</t>
-  </si>
-  <si>
     <t>BH07-HSINCHU</t>
   </si>
   <si>
@@ -708,6 +675,39 @@
   </si>
   <si>
     <t>#CCCC00</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH01</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\Processed-CPT\Hsinchu</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH03</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH04</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH02</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH05</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH06</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH07</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH08</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Input_files\cpt_data_files\RWE-Taiwan</t>
   </si>
 </sst>
 </file>
@@ -1122,8 +1122,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,16 +1219,16 @@
         <v>151</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="F2" s="1" t="b">
         <v>0</v>
@@ -1244,19 +1244,19 @@
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="P2">
         <v>10</v>
@@ -1265,13 +1265,13 @@
         <v>0</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="S2" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -1279,16 +1279,16 @@
         <v>151</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>158</v>
+        <v>182</v>
       </c>
       <c r="F3" s="1" t="b">
         <v>0</v>
@@ -1304,19 +1304,19 @@
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="M3" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="P3">
         <v>10</v>
@@ -1325,7 +1325,7 @@
         <v>0</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -1333,43 +1333,43 @@
         <v>151</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="L4" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="N4" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="F4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="P4">
         <v>10</v>
@@ -1378,7 +1378,7 @@
         <v>0</v>
       </c>
       <c r="R4" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -1386,43 +1386,43 @@
         <v>151</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="L5" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="N5" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="P5">
         <v>10</v>
@@ -1431,13 +1431,13 @@
         <v>0</v>
       </c>
       <c r="R5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="S5" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="T5" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -1445,43 +1445,43 @@
         <v>151</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="L6" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="N6" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="P6">
         <v>10</v>
@@ -1490,7 +1490,7 @@
         <v>0</v>
       </c>
       <c r="R6" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -1498,43 +1498,43 @@
         <v>151</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="L7" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="N7" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="P7">
         <v>10</v>
@@ -1543,13 +1543,13 @@
         <v>0</v>
       </c>
       <c r="R7" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="S7" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="T7" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1557,43 +1557,43 @@
         <v>151</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="L8" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="N8" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="P8">
         <v>10</v>
@@ -1602,7 +1602,7 @@
         <v>0</v>
       </c>
       <c r="R8" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1610,43 +1610,43 @@
         <v>151</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="F9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="L9" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="F9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="N9" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="P9">
         <v>10</v>
@@ -1655,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="R9" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
@@ -1695,7 +1695,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
@@ -1703,7 +1703,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
@@ -1711,7 +1711,7 @@
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
@@ -1719,7 +1719,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
@@ -1727,7 +1727,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B6" t="s">
         <v>29</v>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
@@ -1743,18 +1743,18 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B8" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B9" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed issue with plotting (problem with interactive plot in OCR plot)
</commit_message>
<xml_diff>
--- a/Input_files/Python_Multiple-CPT_Input_Template.xlsx
+++ b/Input_files/Python_Multiple-CPT_Input_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2E35D8-28D6-46B5-88D4-C8C39616895E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD62D430-26B8-44FA-8C8D-C3D84CEBFE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22500" yWindow="3690" windowWidth="18900" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global_variable" sheetId="3" r:id="rId1"/>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="173">
   <si>
     <t>Figure folder path</t>
   </si>
@@ -599,30 +599,12 @@
     <t>SOIL_UNIT-combined.xlsx</t>
   </si>
   <si>
-    <t>Hsinchu-BH1-CPT_processed_data.csv</t>
-  </si>
-  <si>
-    <t>Hsinchu-BH3-CPT_processed_data.csv</t>
-  </si>
-  <si>
     <t>SCPG-combined.xlsx</t>
   </si>
   <si>
     <t>SOIL_PROPERTY-combined.xlsx</t>
   </si>
   <si>
-    <t>Hsinchu-BH4-CPT_processed_data.csv</t>
-  </si>
-  <si>
-    <t>BH01-HSINCHU</t>
-  </si>
-  <si>
-    <t>BH03-HSINCHU</t>
-  </si>
-  <si>
-    <t>BH04-HSINCHU</t>
-  </si>
-  <si>
     <t>Clay</t>
   </si>
   <si>
@@ -641,73 +623,37 @@
     <t>Clayey Sand</t>
   </si>
   <si>
-    <t>Hsinchu-BH2-CPT_processed_data.csv</t>
-  </si>
-  <si>
-    <t>BH02-HSINCHU</t>
-  </si>
-  <si>
-    <t>Hsinchu-BH5-CPT_processed_data.csv</t>
-  </si>
-  <si>
-    <t>BH05-HSINCHU</t>
-  </si>
-  <si>
-    <t>Hsinchu-BH6-CPT_processed_data.csv</t>
-  </si>
-  <si>
-    <t>BH06-HSINCHU</t>
-  </si>
-  <si>
     <t>Silty Clay</t>
   </si>
   <si>
     <t>#99FF99</t>
   </si>
   <si>
-    <t>BH07-HSINCHU</t>
-  </si>
-  <si>
-    <t>BH08-HSINCHU</t>
-  </si>
-  <si>
     <t>Sandy Silt</t>
   </si>
   <si>
     <t>#CCCC00</t>
   </si>
   <si>
+    <t>A2 (2018)</t>
+  </si>
+  <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>A2 (2018)_CPT_processed_data.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\JDN</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\Processed-CPT\JDN</t>
+  </si>
+  <si>
     <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC</t>
   </si>
   <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH01</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\Processed-CPT\Hsinchu</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH03</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH04</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH02</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH05</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH06</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH07</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\RWE-Taiwan\Hsinchu\BH08</t>
-  </si>
-  <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Input_files\cpt_data_files\RWE-Taiwan</t>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Input_files\cpt_data_files\JDN</t>
   </si>
 </sst>
 </file>
@@ -1122,31 +1068,31 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="73.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="65.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.1328125" customWidth="1"/>
+    <col min="4" max="4" width="73.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="65.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.40625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.40625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.1328125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="29" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="22" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.40625" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="14.40625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1214,49 +1160,49 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="F2" s="1" t="b">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="3" t="s">
         <v>152</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>153</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="P2">
         <v>10</v>
@@ -1265,400 +1211,123 @@
         <v>0</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="S2" t="s">
-        <v>160</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1" t="b">
-        <v>0</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.75">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="P3">
-        <v>10</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="P4">
-        <v>10</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="P5">
-        <v>10</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5" t="s">
-        <v>169</v>
-      </c>
-      <c r="S5" t="s">
-        <v>171</v>
-      </c>
-      <c r="T5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="P6">
-        <v>10</v>
-      </c>
-      <c r="Q6">
-        <v>0</v>
-      </c>
-      <c r="R6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="P7">
-        <v>10</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7" t="s">
-        <v>173</v>
-      </c>
-      <c r="S7" t="s">
-        <v>176</v>
-      </c>
-      <c r="T7" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="P8">
-        <v>10</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-      <c r="R8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="P9">
-        <v>10</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="R3" s="3"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.75">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.75">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.75">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.75">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.75">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.75">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.75">
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1677,15 +1346,15 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1693,71 +1362,79 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" s="6" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" s="6" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A4" s="6" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" s="6" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A6" s="6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
       <c r="A7" s="7" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A8" s="7" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A9" s="7" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A10" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B14" s="4"/>
     </row>
   </sheetData>
@@ -1772,20 +1449,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADFFA24-A1D8-4677-A18D-6D80CD0D6B82}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.86328125" customWidth="1"/>
     <col min="4" max="4" width="50" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -1802,7 +1479,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
@@ -1819,7 +1496,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -1836,7 +1513,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -1853,7 +1530,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -1870,7 +1547,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -1887,7 +1564,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -1904,7 +1581,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1921,7 +1598,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -1938,7 +1615,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -1955,7 +1632,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>144</v>
       </c>
@@ -1972,7 +1649,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
         <v>145</v>
       </c>
@@ -1989,7 +1666,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>146</v>
       </c>
@@ -2006,7 +1683,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>147</v>
       </c>
@@ -2023,7 +1700,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -2040,7 +1717,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -2057,7 +1734,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -2074,7 +1751,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -2091,7 +1768,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -2108,7 +1785,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -2125,7 +1802,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -2142,7 +1819,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -2173,15 +1850,15 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.86328125" customWidth="1"/>
+    <col min="5" max="5" width="37.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>102</v>
       </c>
@@ -2201,7 +1878,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -2218,7 +1895,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -2235,7 +1912,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
         <v>122</v>
       </c>
@@ -2252,7 +1929,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -2269,7 +1946,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -2286,7 +1963,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -2303,7 +1980,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -2320,7 +1997,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
         <v>126</v>
       </c>
@@ -2337,7 +2014,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -2369,18 +2046,18 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
+    <col min="6" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>132</v>
       </c>
@@ -2406,7 +2083,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -2432,7 +2109,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A3" s="5">
         <v>0</v>
       </c>
@@ -2452,28 +2129,28 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="D7" s="5"/>
@@ -2495,16 +2172,16 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>131</v>
       </c>
@@ -2527,7 +2204,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2550,7 +2227,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2567,7 +2244,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
       <c r="A4">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Added the statistical module (to be developed)
</commit_message>
<xml_diff>
--- a/Input_files/Python_Multiple-CPT_Input_Template.xlsx
+++ b/Input_files/Python_Multiple-CPT_Input_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD62D430-26B8-44FA-8C8D-C3D84CEBFE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1E6AFD-FB44-4774-BB0F-1F2E46E5E183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15975" yWindow="-14040" windowWidth="19155" windowHeight="10680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global_variable" sheetId="3" r:id="rId1"/>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{82553E4A-3327-467C-AAFA-E37F75DF25F2}">
+    <comment ref="R3" authorId="0" shapeId="0" xr:uid="{140345B7-BFDA-4115-8292-C149C3669EED}">
       <text>
         <r>
           <rPr>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="177">
   <si>
     <t>Figure folder path</t>
   </si>
@@ -644,9 +644,6 @@
     <t>A2 (2018)_CPT_processed_data.csv</t>
   </si>
   <si>
-    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\JDN</t>
-  </si>
-  <si>
     <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\Processed-CPT\JDN</t>
   </si>
   <si>
@@ -654,13 +651,28 @@
   </si>
   <si>
     <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Input_files\cpt_data_files\JDN</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\JDN\C3(2018)_C-5(ITT)</t>
+  </si>
+  <si>
+    <t>C3 (2018)</t>
+  </si>
+  <si>
+    <t>C-5 (ITT)</t>
+  </si>
+  <si>
+    <t>C:\Users\sc\PycharmProjects\SI_processing_automation_SC\Output_files\CPT-fig\JDN\A2 (2018)</t>
+  </si>
+  <si>
+    <t>C3 (2018)_CPT_processed_data.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1068,11 +1080,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G3" sqref="G2:I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
     <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.7265625" bestFit="1" customWidth="1"/>
@@ -1092,7 +1104,7 @@
     <col min="19" max="22" width="14.40625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1160,21 +1172,21 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:22">
       <c r="A2" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>172</v>
-      </c>
       <c r="D2" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="F2" s="1" t="b">
         <v>0</v>
@@ -1215,24 +1227,65 @@
       </c>
       <c r="T2" s="3"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.75">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+    <row r="3" spans="1:22">
+      <c r="A3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="J3" s="2"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="R3" s="3"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.75">
+      <c r="K3" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="P3">
+        <v>10</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="S3" t="s">
+        <v>174</v>
+      </c>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1247,7 +1300,7 @@
       <c r="M4" s="3"/>
       <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:22">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1263,7 +1316,7 @@
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:22">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1279,7 +1332,7 @@
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:22">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1295,7 +1348,7 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:22">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1311,7 +1364,7 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:22">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1327,7 +1380,7 @@
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.75">
+    <row r="24" spans="3:5">
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1349,12 +1402,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -1362,7 +1415,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2">
       <c r="A2" s="6" t="s">
         <v>156</v>
       </c>
@@ -1370,7 +1423,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2">
       <c r="A3" s="6" t="s">
         <v>157</v>
       </c>
@@ -1378,7 +1431,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:2">
       <c r="A4" s="6" t="s">
         <v>158</v>
       </c>
@@ -1386,7 +1439,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2">
       <c r="A5" s="6" t="s">
         <v>159</v>
       </c>
@@ -1394,7 +1447,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:2">
       <c r="A6" s="6" t="s">
         <v>160</v>
       </c>
@@ -1402,7 +1455,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="29.5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:2" ht="29.5">
       <c r="A7" s="7" t="s">
         <v>161</v>
       </c>
@@ -1410,7 +1463,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:2">
       <c r="A8" s="7" t="s">
         <v>162</v>
       </c>
@@ -1418,7 +1471,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:2">
       <c r="A9" s="7" t="s">
         <v>164</v>
       </c>
@@ -1426,7 +1479,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:2">
       <c r="A10" s="7" t="s">
         <v>167</v>
       </c>
@@ -1434,7 +1487,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:2">
       <c r="B14" s="4"/>
     </row>
   </sheetData>
@@ -1453,7 +1506,7 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
     <col min="1" max="1" width="20.86328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.86328125" bestFit="1" customWidth="1"/>
@@ -1462,7 +1515,7 @@
     <col min="5" max="5" width="45" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -1479,7 +1532,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
         <v>53</v>
       </c>
@@ -1496,7 +1549,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>76</v>
       </c>
@@ -1513,7 +1566,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -1530,7 +1583,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -1547,7 +1600,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -1564,7 +1617,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -1581,7 +1634,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1598,7 +1651,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -1615,7 +1668,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>143</v>
       </c>
@@ -1632,7 +1685,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>144</v>
       </c>
@@ -1649,7 +1702,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>145</v>
       </c>
@@ -1666,7 +1719,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>146</v>
       </c>
@@ -1683,7 +1736,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>147</v>
       </c>
@@ -1700,7 +1753,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -1717,7 +1770,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -1734,7 +1787,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>69</v>
       </c>
@@ -1751,7 +1804,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>70</v>
       </c>
@@ -1768,7 +1821,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -1785,7 +1838,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -1802,7 +1855,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -1819,7 +1872,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -1850,7 +1903,7 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
     <col min="1" max="1" width="9.86328125" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="9.86328125" customWidth="1"/>
@@ -1858,7 +1911,7 @@
     <col min="6" max="6" width="25.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>102</v>
       </c>
@@ -1878,7 +1931,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -1895,7 +1948,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1912,7 +1965,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>122</v>
       </c>
@@ -1929,7 +1982,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>55</v>
       </c>
@@ -1946,7 +1999,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -1963,7 +2016,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -1980,7 +2033,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>125</v>
       </c>
@@ -1997,7 +2050,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>126</v>
       </c>
@@ -2014,7 +2067,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -2046,7 +2099,7 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.26953125" bestFit="1" customWidth="1"/>
@@ -2057,7 +2110,7 @@
     <col min="11" max="11" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>132</v>
       </c>
@@ -2083,7 +2136,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:8">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -2109,7 +2162,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:8">
       <c r="A3" s="5">
         <v>0</v>
       </c>
@@ -2129,28 +2182,28 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:8">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:8">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:8">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:8">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="D7" s="5"/>
@@ -2172,7 +2225,7 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="14.75"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.1328125" bestFit="1" customWidth="1"/>
@@ -2181,7 +2234,7 @@
     <col min="7" max="7" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>131</v>
       </c>
@@ -2204,7 +2257,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2227,7 +2280,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2244,7 +2297,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>2</v>
       </c>

</xml_diff>